<commit_message>
focus on exercise items
</commit_message>
<xml_diff>
--- a/byoh/Exercise library.xlsx
+++ b/byoh/Exercise library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\nkragbak.github.io\byoh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DF72A6-3C5C-400F-90C8-128511362215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172426C0-D131-48D1-B628-12B2EABB202D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{78B7EE85-8A37-4CB0-96B7-AD1C2B603977}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{78B7EE85-8A37-4CB0-96B7-AD1C2B603977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,12 +148,6 @@
     <t>Level I: 1 reps</t>
   </si>
   <si>
-    <t>Level IX: 75 reps</t>
-  </si>
-  <si>
-    <t>Level IIX: 50 reps</t>
-  </si>
-  <si>
     <t>Level III: 6 reps</t>
   </si>
   <si>
@@ -419,9 +413,6 @@
     <t>Level II: 30 seconds</t>
   </si>
   <si>
-    <t>Level IV: 90seconds</t>
-  </si>
-  <si>
     <t>Level V: 120 seconds</t>
   </si>
   <si>
@@ -501,6 +492,15 @@
   </si>
   <si>
     <t>CHES</t>
+  </si>
+  <si>
+    <t>Level IV: 90 seconds</t>
+  </si>
+  <si>
+    <t>Level IIX: 30 reps</t>
+  </si>
+  <si>
+    <t>Level IX: 60 reps</t>
   </si>
 </sst>
 </file>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE1469C-723F-446B-9820-DC751799AA0C}">
   <dimension ref="B3:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1041,7 +1041,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
@@ -1050,7 +1050,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1064,7 +1064,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1074,13 +1074,13 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3"/>
       <c r="F10" s="6"/>
@@ -1088,7 +1088,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K10" s="6"/>
     </row>
@@ -1098,7 +1098,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1112,7 +1112,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K12" s="6"/>
     </row>
@@ -1122,7 +1122,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1136,7 +1136,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="K14" s="6"/>
     </row>
@@ -1146,7 +1146,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1177,7 +1177,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1190,7 +1190,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1200,7 +1200,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -1213,7 +1213,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K20" s="6"/>
     </row>
@@ -1223,7 +1223,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -1232,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1242,7 +1242,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="K23" s="6"/>
     </row>
@@ -1255,7 +1255,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -1265,7 +1265,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -1274,22 +1274,22 @@
         <v>5</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
@@ -1298,7 +1298,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K27" s="6"/>
     </row>
@@ -1311,19 +1311,19 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K29" s="6"/>
     </row>
@@ -1336,7 +1336,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K30" s="6"/>
     </row>
@@ -1346,7 +1346,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -1359,7 +1359,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1369,7 +1369,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -1379,170 +1379,170 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K34" s="6"/>
     </row>
     <row r="35" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>0</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F37" s="6"/>
       <c r="J37" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F38" s="6"/>
       <c r="J38" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F39" s="6"/>
       <c r="J39" s="6" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="6:11" x14ac:dyDescent="0.35">
       <c r="J40" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F41" s="6"/>
       <c r="J41" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="6:11" x14ac:dyDescent="0.35">
       <c r="J42" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="6:11" x14ac:dyDescent="0.35">
       <c r="J43" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="6:11" x14ac:dyDescent="0.35">
       <c r="J44" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="6:11" x14ac:dyDescent="0.35">
       <c r="J45" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="6:11" ht="29" x14ac:dyDescent="0.35">
       <c r="F46" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>0</v>
       </c>
       <c r="H46" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J46" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="47" spans="6:11" x14ac:dyDescent="0.35">
       <c r="J47" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F48" s="6"/>
       <c r="J48" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F49" s="6"/>
       <c r="J49" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F50" s="6"/>
       <c r="J50" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F51" s="6"/>
       <c r="J51" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F52" s="6"/>
       <c r="J52" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F53" s="6"/>
       <c r="J53" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F54" s="6"/>
       <c r="J54" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F55" s="6"/>
       <c r="J55" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F58" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F59" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F60" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F61" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="6:10" x14ac:dyDescent="0.35">
@@ -1550,47 +1550,47 @@
     </row>
     <row r="63" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F63" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F64" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F65" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F66" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G67" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G68" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G69" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G70" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G71" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>